<commit_message>
update load list admin
</commit_message>
<xml_diff>
--- a/excel/turn 15.14.38.xlsx
+++ b/excel/turn 15.14.38.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>turn</t>
   </si>
@@ -19,49 +19,25 @@
     <t>time_begin</t>
   </si>
   <si>
-    <t>adfd</t>
-  </si>
-  <si>
     <t>7h00</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>7h30</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>8h00</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>8h30</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>9h00</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>9h30</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>10h00</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
   <si>
     <t>10h30</t>
@@ -147,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -158,21 +134,6 @@
     <border>
       <left style="thin">
         <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -193,7 +154,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -230,21 +191,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -258,31 +204,31 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1415,249 +1361,249 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.65" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s" s="4">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="D1" t="s" s="4">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="14.45" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" t="s" s="8">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="14.45" customHeight="1">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" ht="14.45" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" t="s" s="8">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="14.45" customHeight="1">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="14.45" customHeight="1">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" ht="14.45" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" t="s" s="8">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="14.45" customHeight="1">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="14.45" customHeight="1">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" ht="14.45" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" t="s" s="8">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="14.45" customHeight="1">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="8">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="14.45" customHeight="1">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" ht="14.45" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" t="s" s="8">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="14.45" customHeight="1">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D6" t="s" s="8">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="14.45" customHeight="1">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" ht="14.45" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" t="s" s="8">
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="14.45" customHeight="1">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D7" t="s" s="8">
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" ht="14.45" customHeight="1">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" ht="14.45" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" t="s" s="8">
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" ht="14.45" customHeight="1">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D8" t="s" s="8">
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" ht="14.45" customHeight="1">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" ht="14.45" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" t="s" s="8">
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" ht="14.45" customHeight="1">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D9" t="s" s="8">
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" ht="14.45" customHeight="1">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" ht="14.45" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="10">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s" s="8">
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" ht="14.45" customHeight="1">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" ht="14.45" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="10">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s" s="8">
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" ht="14.45" customHeight="1">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" ht="14.45" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s" s="8">
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" ht="14.45" customHeight="1">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" ht="14.45" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="10">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s" s="8">
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" ht="14.45" customHeight="1">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" ht="14.45" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="10">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" ht="14.45" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="10">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" ht="14.45" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" ht="14.45" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="10">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" ht="14.45" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" ht="14.45" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="10">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" ht="14.45" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="10">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s" s="8">
-        <v>28</v>
-      </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" ht="14.45" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="10">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s" s="8">
-        <v>29</v>
-      </c>
-      <c r="E21" s="9"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" ht="14.45" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" ht="14.45" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>